<commit_message>
BCDatHang: add column {TienChietKhau, TienThue}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoDatHang/Teamplate_BaoCaoDatHangChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoDatHang/Teamplate_BaoCaoDatHangChiTiet.xlsx
@@ -17,236 +17,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <r>
-      <t xml:space="preserve">Mã chứng từ
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(1)</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Tổng cộng:</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Ngày chứng từ
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(2)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Khách hàng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(3)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mã hàng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(4)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tên hàng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(5)</t>
-    </r>
-  </si>
-  <si>
     <t>BÁO CÁO ĐẶT HÀNG CHI TIẾT</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Đơn vị tính
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(6)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lô hàng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(7)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Số lượng đặt
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(8)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Thành tiền
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(9)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Giảm giá HD
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(10)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Giá trị đặt
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(11 = 9-10)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Số lượng nhận
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(12)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Nhân viên
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(13)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ghi chú
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(14)</t>
-    </r>
+    <t>Mã chứng từ</t>
+  </si>
+  <si>
+    <t>Ngày chứng từ</t>
+  </si>
+  <si>
+    <t>Khách hàng</t>
+  </si>
+  <si>
+    <t>Mã hàng</t>
+  </si>
+  <si>
+    <t>Tên hàng</t>
+  </si>
+  <si>
+    <t>Đơn vị tính</t>
+  </si>
+  <si>
+    <t>Lô hàng</t>
+  </si>
+  <si>
+    <t>Số lượng đặt</t>
+  </si>
+  <si>
+    <t>Đơn giá</t>
+  </si>
+  <si>
+    <t>Chiết khấu</t>
+  </si>
+  <si>
+    <t>Thành tiền</t>
+  </si>
+  <si>
+    <t>Giảm giá HD</t>
+  </si>
+  <si>
+    <t>Giá trị đặt</t>
+  </si>
+  <si>
+    <t>Số lượng nhận</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Tiền thuế</t>
   </si>
 </sst>
 </file>
@@ -767,11 +594,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,16 +610,18 @@
     <col min="6" max="6" width="21.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" style="4" customWidth="1"/>
     <col min="8" max="9" width="16.42578125" style="20" customWidth="1"/>
-    <col min="10" max="11" width="14.7109375" style="20" customWidth="1"/>
-    <col min="12" max="12" width="18" style="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.85546875" style="13" customWidth="1"/>
-    <col min="14" max="14" width="25.85546875" style="17" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17.7109375" style="20" customWidth="1"/>
+    <col min="11" max="12" width="16.42578125" style="20" customWidth="1"/>
+    <col min="13" max="14" width="14.7109375" style="20" customWidth="1"/>
+    <col min="15" max="15" width="18" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.85546875" style="13" customWidth="1"/>
+    <col min="17" max="17" width="25.85546875" style="17" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -807,9 +636,12 @@
       <c r="L1" s="24"/>
       <c r="M1" s="24"/>
       <c r="N1" s="24"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="25"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -824,25 +656,28 @@
       <c r="L2" s="25"/>
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
     </row>
-    <row r="4" spans="1:15" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>7</v>
@@ -863,16 +698,25 @@
         <v>12</v>
       </c>
       <c r="L4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="16"/>
       <c r="C5" s="3"/>
@@ -885,10 +729,13 @@
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="18"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="18"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="16"/>
       <c r="C6" s="3"/>
@@ -901,10 +748,13 @@
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
       <c r="L6" s="22"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="18"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="18"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="16"/>
       <c r="C7" s="3"/>
@@ -917,10 +767,13 @@
       <c r="J7" s="22"/>
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="18"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="18"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="16"/>
       <c r="C8" s="3"/>
@@ -933,10 +786,13 @@
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
       <c r="L8" s="22"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="18"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="18"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="16"/>
       <c r="C9" s="3"/>
@@ -949,10 +805,13 @@
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
       <c r="L9" s="22"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="18"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="18"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="16"/>
       <c r="C10" s="3"/>
@@ -965,10 +824,13 @@
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="18"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="18"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="16"/>
       <c r="C11" s="3"/>
@@ -981,10 +843,13 @@
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
       <c r="L11" s="22"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="18"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="18"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="16"/>
       <c r="C12" s="3"/>
@@ -997,10 +862,13 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="18"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="18"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
       <c r="C13" s="3"/>
@@ -1013,10 +881,13 @@
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="18"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="22"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="18"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="16"/>
       <c r="C14" s="3"/>
@@ -1029,10 +900,13 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="18"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="16"/>
       <c r="C15" s="3"/>
@@ -1045,10 +919,13 @@
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
       <c r="L15" s="22"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="18"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="18"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="16"/>
       <c r="C16" s="3"/>
@@ -1061,10 +938,13 @@
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
       <c r="L16" s="22"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="18"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="18"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="16"/>
       <c r="C17" s="3"/>
@@ -1077,10 +957,13 @@
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
       <c r="L17" s="22"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="18"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="18"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
       <c r="C18" s="3"/>
@@ -1093,10 +976,13 @@
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
       <c r="L18" s="22"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="18"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="18"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="16"/>
       <c r="C19" s="3"/>
@@ -1109,10 +995,13 @@
       <c r="J19" s="22"/>
       <c r="K19" s="22"/>
       <c r="L19" s="22"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="18"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="18"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="16"/>
       <c r="C20" s="3"/>
@@ -1125,10 +1014,13 @@
       <c r="J20" s="22"/>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="18"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="18"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="16"/>
       <c r="C21" s="3"/>
@@ -1141,10 +1033,13 @@
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="18"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="18"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="16"/>
       <c r="C22" s="3"/>
@@ -1157,10 +1052,13 @@
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="18"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="18"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="16"/>
       <c r="C23" s="3"/>
@@ -1173,10 +1071,13 @@
       <c r="J23" s="22"/>
       <c r="K23" s="22"/>
       <c r="L23" s="22"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="18"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="18"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="16"/>
       <c r="C24" s="3"/>
@@ -1189,10 +1090,13 @@
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
       <c r="L24" s="22"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="18"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="18"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="16"/>
       <c r="C25" s="3"/>
@@ -1205,10 +1109,13 @@
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
       <c r="L25" s="22"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="18"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="18"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="16"/>
       <c r="C26" s="3"/>
@@ -1221,10 +1128,13 @@
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="18"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="18"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="16"/>
       <c r="C27" s="3"/>
@@ -1237,10 +1147,13 @@
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="18"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="18"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="16"/>
       <c r="C28" s="3"/>
@@ -1253,12 +1166,15 @@
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="18"/>
-    </row>
-    <row r="29" spans="1:14" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="18"/>
+    </row>
+    <row r="29" spans="1:17" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="27"/>
@@ -1270,10 +1186,7 @@
         <f>SUM(H$5:H28)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="23">
-        <f>SUM(I$5:I28)</f>
-        <v>0</v>
-      </c>
+      <c r="I29" s="23"/>
       <c r="J29" s="23">
         <f>SUM(J$5:J28)</f>
         <v>0</v>
@@ -1286,13 +1199,25 @@
         <f>SUM(L$5:L28)</f>
         <v>0</v>
       </c>
-      <c r="M29" s="12"/>
-      <c r="N29" s="19"/>
+      <c r="M29" s="23">
+        <f>SUM(M$5:M28)</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="23">
+        <f>SUM(N$5:N28)</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="23">
+        <f>SUM(O$5:O28)</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
     <mergeCell ref="A29:G29"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>

</xml_diff>